<commit_message>
checks trial associated with sound
</commit_message>
<xml_diff>
--- a/data/fNIRSandGerbils.xlsx
+++ b/data/fNIRSandGerbils.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Experiments\fNIRSandGerbils\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF54A7FB-DCDB-4258-A362-D0B6A6168F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D53AF44E-4C63-4895-9BF6-C96A9BDC5969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{E27CA675-299A-4EB1-A046-89C40DE47D7A}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="17400" xr2:uid="{E27CA675-299A-4EB1-A046-89C40DE47D7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="266">
   <si>
     <t>S</t>
   </si>
@@ -831,6 +831,9 @@
   </si>
   <si>
     <t>D:\Experiments\fNIRSandGerbils\stim\s_longtest2\unscrambled\8_unscrambled.wav</t>
+  </si>
+  <si>
+    <t>perfectdata</t>
   </si>
 </sst>
 </file>
@@ -1183,13 +1186,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E945CDA-0894-470B-A916-C9F7C84C6ED4}">
-  <dimension ref="A1:M255"/>
+  <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="G264" sqref="G264"/>
+    <sheetView tabSelected="1" topLeftCell="A147" workbookViewId="0">
+      <selection activeCell="G170" sqref="G170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="7" max="7" width="104" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -10203,6 +10210,628 @@
         <v>8.7200000000000006</v>
       </c>
     </row>
+    <row r="256" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A256" t="s">
+        <v>265</v>
+      </c>
+      <c r="B256">
+        <v>1</v>
+      </c>
+      <c r="D256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>265</v>
+      </c>
+      <c r="B257">
+        <f>B256+1</f>
+        <v>2</v>
+      </c>
+      <c r="D257">
+        <f>D256+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A258" t="s">
+        <v>265</v>
+      </c>
+      <c r="B258">
+        <f t="shared" ref="B258:D305" si="0">B257+1</f>
+        <v>3</v>
+      </c>
+      <c r="D258">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>265</v>
+      </c>
+      <c r="B259">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D259">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" t="s">
+        <v>265</v>
+      </c>
+      <c r="B260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D260">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>265</v>
+      </c>
+      <c r="B261">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D261">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" t="s">
+        <v>265</v>
+      </c>
+      <c r="B262">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D262">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>265</v>
+      </c>
+      <c r="B263">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D263">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" t="s">
+        <v>265</v>
+      </c>
+      <c r="B264">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D264">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>265</v>
+      </c>
+      <c r="B265">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D265">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
+        <v>265</v>
+      </c>
+      <c r="B266">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D266">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>265</v>
+      </c>
+      <c r="B267">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D267">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
+        <v>265</v>
+      </c>
+      <c r="B268">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D268">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>265</v>
+      </c>
+      <c r="B269">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D269">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>265</v>
+      </c>
+      <c r="B270">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D270">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>265</v>
+      </c>
+      <c r="B271">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D271">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
+        <v>265</v>
+      </c>
+      <c r="B272">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D272">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>265</v>
+      </c>
+      <c r="B273">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D273">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
+        <v>265</v>
+      </c>
+      <c r="B274">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D274">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>265</v>
+      </c>
+      <c r="B275">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D275">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A276" t="s">
+        <v>265</v>
+      </c>
+      <c r="B276">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D276">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>265</v>
+      </c>
+      <c r="B277">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D277">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
+        <v>265</v>
+      </c>
+      <c r="B278">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D278">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>265</v>
+      </c>
+      <c r="B279">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D279">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
+        <v>265</v>
+      </c>
+      <c r="B280">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D280">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>265</v>
+      </c>
+      <c r="B281">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D281">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
+        <v>265</v>
+      </c>
+      <c r="B282">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D282">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>265</v>
+      </c>
+      <c r="B283">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D283">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
+        <v>265</v>
+      </c>
+      <c r="B284">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D284">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>265</v>
+      </c>
+      <c r="B285">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D285">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
+        <v>265</v>
+      </c>
+      <c r="B286">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D286">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>265</v>
+      </c>
+      <c r="B287">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D287">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
+        <v>265</v>
+      </c>
+      <c r="B288">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D288">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>265</v>
+      </c>
+      <c r="B289">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D289">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A290" t="s">
+        <v>265</v>
+      </c>
+      <c r="B290">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D290">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>265</v>
+      </c>
+      <c r="B291">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D291">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>265</v>
+      </c>
+      <c r="B292">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D292">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>265</v>
+      </c>
+      <c r="B293">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D293">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
+        <v>265</v>
+      </c>
+      <c r="B294">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D294">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>265</v>
+      </c>
+      <c r="B295">
+        <f>B294+1</f>
+        <v>40</v>
+      </c>
+      <c r="D295">
+        <f>D294+1</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>265</v>
+      </c>
+      <c r="B296">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D296">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>265</v>
+      </c>
+      <c r="B297">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D297">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>265</v>
+      </c>
+      <c r="B298">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D298">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>265</v>
+      </c>
+      <c r="B299">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D299">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A300" t="s">
+        <v>265</v>
+      </c>
+      <c r="B300">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D300">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>265</v>
+      </c>
+      <c r="B301">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D301">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A302" t="s">
+        <v>265</v>
+      </c>
+      <c r="B302">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D302">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>265</v>
+      </c>
+      <c r="B303">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D303">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>